<commit_message>
The quick brown fox jumps over the lazy dog.
</commit_message>
<xml_diff>
--- a/Data/Ex02Excel.xlsx
+++ b/Data/Ex02Excel.xlsx
@@ -59,7 +59,7 @@
     <t>ThisIsAValidEmail@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">健康美 </t>
+    <t>Incorrect</t>
   </si>
   <si>
     <t>An email address required.</t>
@@ -1334,7 +1334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="22.35" customHeight="1">
+    <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="5">
         <v>9</v>
       </c>

</xml_diff>